<commit_message>
Automation for CS Portal
CSP 1.15 - Bug fix
</commit_message>
<xml_diff>
--- a/resources/excels/CD.xlsx
+++ b/resources/excels/CD.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11012"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2394650\IdeaProjects\cs-portal-automation_selenium1\resources\excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a13221514/IdeaProjects/cs-portal-automation_selenium/resources/excels/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBED29ED-35DA-4843-AC25-06765552C7E4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="34680" windowHeight="9255" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
@@ -36,7 +37,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'FTRTickets-Reg'!$A$1:$F$126</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'SLA Configuration'!$A$1:$R$1</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -46,12 +47,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Rahul Gupta</author>
   </authors>
   <commentList>
-    <comment ref="AV1" authorId="0" shapeId="0">
+    <comment ref="AV1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -75,7 +76,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AW1" authorId="0" shapeId="0">
+    <comment ref="AW1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
       <text>
         <r>
           <rPr>
@@ -99,7 +100,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AX1" authorId="0" shapeId="0">
+    <comment ref="AX1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
       <text>
         <r>
           <rPr>
@@ -124,7 +125,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AY1" authorId="0" shapeId="0">
+    <comment ref="AY1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000004000000}">
       <text>
         <r>
           <rPr>
@@ -148,7 +149,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AZ1" authorId="0" shapeId="0">
+    <comment ref="AZ1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000005000000}">
       <text>
         <r>
           <rPr>
@@ -177,12 +178,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Rahul Gupta</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
       <text>
         <r>
           <rPr>
@@ -206,7 +207,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000002000000}">
       <text>
         <r>
           <rPr>
@@ -235,12 +236,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Rahul Gupta</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000001000000}">
       <text>
         <r>
           <rPr>
@@ -264,7 +265,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000002000000}">
       <text>
         <r>
           <rPr>
@@ -288,7 +289,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000003000000}">
       <text>
         <r>
           <rPr>
@@ -313,7 +314,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000004000000}">
       <text>
         <r>
           <rPr>
@@ -337,7 +338,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000005000000}">
       <text>
         <r>
           <rPr>
@@ -366,12 +367,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Rahul Gupta</author>
   </authors>
   <commentList>
-    <comment ref="AV1" authorId="0" shapeId="0">
+    <comment ref="AV1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000001000000}">
       <text>
         <r>
           <rPr>
@@ -395,7 +396,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AW1" authorId="0" shapeId="0">
+    <comment ref="AW1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000002000000}">
       <text>
         <r>
           <rPr>
@@ -419,7 +420,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AX1" authorId="0" shapeId="0">
+    <comment ref="AX1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000003000000}">
       <text>
         <r>
           <rPr>
@@ -444,7 +445,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AY1" authorId="0" shapeId="0">
+    <comment ref="AY1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000004000000}">
       <text>
         <r>
           <rPr>
@@ -468,7 +469,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AZ1" authorId="0" shapeId="0">
+    <comment ref="AZ1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000005000000}">
       <text>
         <r>
           <rPr>
@@ -497,7 +498,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3370" uniqueCount="1115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3383" uniqueCount="1120">
   <si>
     <t>loginAuuid</t>
   </si>
@@ -3846,12 +3847,31 @@
   </si>
   <si>
     <t>Security Deposit</t>
+  </si>
+  <si>
+    <t>More Airtel Money Secondary History</t>
+  </si>
+  <si>
+    <t>Amount
+(USD)</t>
+  </si>
+  <si>
+    <t>Service Charge
+(USD)</t>
+  </si>
+  <si>
+    <t>Pre balance
+(USD)</t>
+  </si>
+  <si>
+    <t>Post balance
+(USD)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="15">
     <font>
       <sz val="11"/>
@@ -4175,11 +4195,11 @@
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal 3" xfId="2"/>
-    <cellStyle name="Normal 4" xfId="3"/>
-    <cellStyle name="Normal 4 2" xfId="4"/>
-    <cellStyle name="Normal 4 3" xfId="5"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 4" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 4 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 4 3" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
@@ -4265,7 +4285,7 @@
         <xdr:cNvPr id="3" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4308,7 +4328,7 @@
         <xdr:cNvPr id="4" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4351,7 +4371,7 @@
         <xdr:cNvPr id="5" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4394,7 +4414,7 @@
         <xdr:cNvPr id="6" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4437,7 +4457,7 @@
         <xdr:cNvPr id="7" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4732,20 +4752,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="18.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="18.1640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75">
+    <row r="1" spans="1:17" ht="16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4888,17 +4908,17 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" activeCellId="1" sqref="E9 C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="25.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="25.83203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -4912,7 +4932,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75">
+    <row r="2" spans="1:3" ht="16">
       <c r="A2" s="16" t="s">
         <v>62</v>
       </c>
@@ -4923,7 +4943,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75">
+    <row r="3" spans="1:3" ht="16">
       <c r="A3" s="16" t="s">
         <v>63</v>
       </c>
@@ -4934,7 +4954,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75">
+    <row r="4" spans="1:3" ht="16">
       <c r="A4" s="16" t="s">
         <v>64</v>
       </c>
@@ -4945,7 +4965,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75">
+    <row r="5" spans="1:3" ht="16">
       <c r="A5" s="16" t="s">
         <v>65</v>
       </c>
@@ -4956,7 +4976,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75">
+    <row r="6" spans="1:3" ht="16">
       <c r="B6" s="17" t="s">
         <v>133</v>
       </c>
@@ -4964,7 +4984,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75">
+    <row r="7" spans="1:3" ht="16">
       <c r="B7" s="17" t="s">
         <v>134</v>
       </c>
@@ -4972,7 +4992,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75">
+    <row r="8" spans="1:3" ht="16">
       <c r="B8" s="17" t="s">
         <v>135</v>
       </c>
@@ -4996,22 +5016,22 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75">
+    <row r="1" spans="1:4" ht="16">
       <c r="A1" s="18" t="s">
         <v>48</v>
       </c>
@@ -5103,21 +5123,21 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.1640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75">
+    <row r="1" spans="1:3" ht="16">
       <c r="A1" s="4" t="s">
         <v>53</v>
       </c>
@@ -5128,7 +5148,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75">
+    <row r="2" spans="1:3" ht="16">
       <c r="A2" s="8" t="s">
         <v>56</v>
       </c>
@@ -5137,7 +5157,7 @@
       </c>
       <c r="C2" s="6"/>
     </row>
-    <row r="3" spans="1:3" ht="15.75">
+    <row r="3" spans="1:3" ht="16">
       <c r="A3" s="9" t="s">
         <v>57</v>
       </c>
@@ -5146,7 +5166,7 @@
       </c>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:3" ht="15.75">
+    <row r="4" spans="1:3" ht="16">
       <c r="A4" s="9" t="s">
         <v>59</v>
       </c>
@@ -5155,7 +5175,7 @@
       </c>
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:3" ht="15.75">
+    <row r="5" spans="1:3" ht="16">
       <c r="A5" s="9" t="s">
         <v>60</v>
       </c>
@@ -5164,7 +5184,7 @@
       </c>
       <c r="C5" s="5"/>
     </row>
-    <row r="6" spans="1:3" ht="15.75">
+    <row r="6" spans="1:3" ht="16">
       <c r="A6" s="9" t="s">
         <v>61</v>
       </c>
@@ -5181,17 +5201,17 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="35.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" width="35.33203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="16384" width="9.1640625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -5247,21 +5267,21 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="15.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="42.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="9.1640625" style="1"/>
+    <col min="2" max="2" width="15.33203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="42.5" style="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="23" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="31.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="5" width="31.6640625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -5287,31 +5307,31 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" style="27" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" style="27" customWidth="1"/>
-    <col min="6" max="7" width="11.42578125" style="27" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" style="27" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" style="27" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="27" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" style="27" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" style="27" customWidth="1"/>
+    <col min="6" max="7" width="11.5" style="27" customWidth="1"/>
+    <col min="8" max="8" width="12.5" style="27" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" style="27" customWidth="1"/>
+    <col min="10" max="10" width="11.5" style="27" customWidth="1"/>
     <col min="11" max="11" width="12" style="27" customWidth="1"/>
-    <col min="12" max="12" width="13.28515625" style="27" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" style="27" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
+    <col min="12" max="12" width="13.33203125" style="27" customWidth="1"/>
+    <col min="13" max="13" width="13.5" style="27" customWidth="1"/>
+    <col min="14" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" ht="17">
       <c r="A1" s="1" t="s">
         <v>871</v>
       </c>
@@ -5352,7 +5372,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="141.75">
+    <row r="2" spans="1:13" ht="153">
       <c r="A2" s="1" t="s">
         <v>884</v>
       </c>
@@ -5387,23 +5407,23 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="12.42578125" style="1" customWidth="1"/>
-    <col min="4" max="6" width="9.140625" style="1"/>
+    <col min="1" max="1" width="15.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="1"/>
+    <col min="3" max="3" width="12.5" style="1" customWidth="1"/>
+    <col min="4" max="6" width="9.1640625" style="1"/>
     <col min="7" max="7" width="16" style="1" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="21.85546875" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="8" max="8" width="17.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="21.83203125" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -5639,16 +5659,16 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75">
+    <row r="1" spans="1:3" ht="16">
       <c r="A1" s="18" t="s">
         <v>869</v>
       </c>
@@ -5659,7 +5679,7 @@
         <v>1021</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75">
+    <row r="2" spans="1:3" ht="16">
       <c r="A2" s="19" t="s">
         <v>136</v>
       </c>
@@ -5670,7 +5690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75">
+    <row r="3" spans="1:3" ht="16">
       <c r="A3" s="19" t="s">
         <v>137</v>
       </c>
@@ -5681,7 +5701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75">
+    <row r="4" spans="1:3" ht="16">
       <c r="A4" s="19" t="s">
         <v>130</v>
       </c>
@@ -5698,22 +5718,22 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" style="20" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" style="20" customWidth="1"/>
-    <col min="3" max="3" width="51.140625" style="20" customWidth="1"/>
-    <col min="4" max="16384" width="10.85546875" style="20"/>
+    <col min="1" max="1" width="24.5" style="20" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" style="20" customWidth="1"/>
+    <col min="3" max="3" width="51.1640625" style="20" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75">
+    <row r="1" spans="1:3" ht="17">
       <c r="A1" s="38" t="s">
         <v>1022</v>
       </c>
@@ -5724,7 +5744,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75">
+    <row r="2" spans="1:3" ht="17">
       <c r="A2" s="38" t="s">
         <v>1025</v>
       </c>
@@ -5735,7 +5755,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="47.25">
+    <row r="3" spans="1:3" ht="51">
       <c r="A3" s="38" t="s">
         <v>1028</v>
       </c>
@@ -5746,7 +5766,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75">
+    <row r="4" spans="1:3" ht="17">
       <c r="A4" s="38" t="s">
         <v>1031</v>
       </c>
@@ -5757,7 +5777,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75">
+    <row r="5" spans="1:3" ht="17">
       <c r="A5" s="38" t="s">
         <v>1034</v>
       </c>
@@ -5768,7 +5788,7 @@
         <v>1036</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="31.5">
+    <row r="6" spans="1:3" ht="34">
       <c r="A6" s="38" t="s">
         <v>1037</v>
       </c>
@@ -5777,7 +5797,7 @@
       </c>
       <c r="C6" s="39"/>
     </row>
-    <row r="7" spans="1:3" ht="31.5">
+    <row r="7" spans="1:3" ht="17">
       <c r="A7" s="38" t="s">
         <v>1039</v>
       </c>
@@ -5788,7 +5808,7 @@
         <v>1041</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="31.5">
+    <row r="8" spans="1:3" ht="17">
       <c r="A8" s="38" t="s">
         <v>1042</v>
       </c>
@@ -5799,7 +5819,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="31.5">
+    <row r="9" spans="1:3" ht="17">
       <c r="A9" s="38" t="s">
         <v>1045</v>
       </c>
@@ -5810,7 +5830,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="47.25">
+    <row r="10" spans="1:3" ht="34">
       <c r="A10" s="38" t="s">
         <v>1048</v>
       </c>
@@ -5821,7 +5841,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="31.5">
+    <row r="11" spans="1:3" ht="17">
       <c r="A11" s="38" t="s">
         <v>1051</v>
       </c>
@@ -5832,7 +5852,7 @@
         <v>1053</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75">
+    <row r="12" spans="1:3" ht="17">
       <c r="A12" s="38" t="s">
         <v>1054</v>
       </c>
@@ -5843,7 +5863,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75">
+    <row r="13" spans="1:3" ht="17">
       <c r="A13" s="38" t="s">
         <v>1057</v>
       </c>
@@ -5852,7 +5872,7 @@
       </c>
       <c r="C13" s="39"/>
     </row>
-    <row r="14" spans="1:3" ht="31.5">
+    <row r="14" spans="1:3" ht="17">
       <c r="A14" s="38" t="s">
         <v>1059</v>
       </c>
@@ -5861,7 +5881,7 @@
       </c>
       <c r="C14" s="39"/>
     </row>
-    <row r="15" spans="1:3" ht="15.75">
+    <row r="15" spans="1:3" ht="17">
       <c r="A15" s="38" t="s">
         <v>1061</v>
       </c>
@@ -5878,20 +5898,20 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22" style="29" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="29"/>
-    <col min="3" max="3" width="15.85546875" style="29" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" style="29" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="29"/>
+    <col min="2" max="2" width="9.1640625" style="29"/>
+    <col min="3" max="3" width="15.83203125" style="29" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" style="29" customWidth="1"/>
+    <col min="5" max="16384" width="9.1640625" style="29"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -5929,7 +5949,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75">
+    <row r="2" spans="1:11" ht="16">
       <c r="A2" s="10" t="s">
         <v>136</v>
       </c>
@@ -5950,7 +5970,7 @@
       <c r="J2" s="28"/>
       <c r="K2" s="28"/>
     </row>
-    <row r="3" spans="1:11" ht="15.75">
+    <row r="3" spans="1:11" ht="16">
       <c r="A3" s="10" t="s">
         <v>131</v>
       </c>
@@ -5971,7 +5991,7 @@
       <c r="J3" s="28"/>
       <c r="K3" s="28"/>
     </row>
-    <row r="4" spans="1:11" ht="15.75">
+    <row r="4" spans="1:11" ht="16">
       <c r="A4" s="10" t="s">
         <v>135</v>
       </c>
@@ -5999,19 +6019,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75">
+    <row r="1" spans="1:1" ht="16">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
@@ -6052,25 +6072,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="33.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.1640625" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6115,7 +6135,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" ht="16">
       <c r="A2" s="12" t="s">
         <v>68</v>
       </c>
@@ -6169,7 +6189,7 @@
       <c r="L3" s="12"/>
       <c r="M3" s="12"/>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" ht="16">
       <c r="A4" s="12" t="s">
         <v>91</v>
       </c>
@@ -6443,7 +6463,7 @@
       <c r="L13" s="12"/>
       <c r="M13" s="12"/>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" ht="16">
       <c r="A14" s="31" t="s">
         <v>943</v>
       </c>
@@ -6588,7 +6608,7 @@
       <c r="L18" s="12"/>
       <c r="M18" s="12"/>
     </row>
-    <row r="19" spans="1:13" ht="45">
+    <row r="19" spans="1:13" ht="32">
       <c r="A19" s="31" t="s">
         <v>978</v>
       </c>
@@ -6629,119 +6649,133 @@
         <v>983</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" ht="32">
       <c r="A20" s="31" t="s">
+        <v>1115</v>
+      </c>
+      <c r="B20" s="32" t="s">
+        <v>1116</v>
+      </c>
+      <c r="C20" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" s="31" t="s">
+        <v>979</v>
+      </c>
+      <c r="E20" s="31" t="s">
+        <v>980</v>
+      </c>
+      <c r="F20" s="31" t="s">
+        <v>981</v>
+      </c>
+      <c r="G20" s="31" t="s">
+        <v>982</v>
+      </c>
+      <c r="H20" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="I20" s="33" t="s">
+        <v>1117</v>
+      </c>
+      <c r="J20" s="33" t="s">
+        <v>1118</v>
+      </c>
+      <c r="K20" s="33" t="s">
+        <v>1119</v>
+      </c>
+      <c r="L20" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="M20" s="31" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" s="31" t="s">
         <v>984</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B21" s="12" t="s">
         <v>985</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C21" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="D20" s="31" t="s">
+      <c r="D21" s="31" t="s">
         <v>986</v>
       </c>
-      <c r="E20" s="31" t="s">
+      <c r="E21" s="31" t="s">
         <v>987</v>
       </c>
-      <c r="F20" s="31" t="s">
+      <c r="F21" s="31" t="s">
         <v>988</v>
       </c>
-      <c r="G20" s="31" t="s">
+      <c r="G21" s="31" t="s">
         <v>989</v>
       </c>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="12"/>
-      <c r="L20" s="12"/>
-      <c r="M20" s="12"/>
-    </row>
-    <row r="21" spans="1:13">
-      <c r="A21" s="12" t="s">
-        <v>1064</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>1065</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>1066</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>1067</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>964</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="G21" s="12" t="s">
-        <v>1068</v>
-      </c>
-      <c r="H21" s="12" t="s">
-        <v>1069</v>
-      </c>
-      <c r="I21" s="12" t="s">
-        <v>1070</v>
-      </c>
-      <c r="J21" s="12" t="s">
-        <v>1071</v>
-      </c>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
       <c r="K21" s="12"/>
       <c r="L21" s="12"/>
       <c r="M21" s="12"/>
     </row>
     <row r="22" spans="1:13">
       <c r="A22" s="12" t="s">
-        <v>1072</v>
+        <v>1064</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>1073</v>
+        <v>1065</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>1074</v>
+        <v>1066</v>
       </c>
       <c r="D22" s="12" t="s">
+        <v>1067</v>
+      </c>
+      <c r="E22" s="12" t="s">
         <v>964</v>
       </c>
-      <c r="E22" s="12" t="s">
+      <c r="F22" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="F22" s="12" t="s">
-        <v>1075</v>
-      </c>
       <c r="G22" s="12" t="s">
-        <v>892</v>
-      </c>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
+        <v>1068</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>1069</v>
+      </c>
+      <c r="I22" s="12" t="s">
+        <v>1070</v>
+      </c>
+      <c r="J22" s="12" t="s">
+        <v>1071</v>
+      </c>
       <c r="K22" s="12"/>
       <c r="L22" s="12"/>
       <c r="M22" s="12"/>
     </row>
-    <row r="23" spans="1:13" ht="16.5">
-      <c r="A23" s="46" t="s">
-        <v>1093</v>
-      </c>
-      <c r="B23" s="31" t="s">
-        <v>1094</v>
-      </c>
-      <c r="C23" s="31" t="s">
-        <v>1095</v>
-      </c>
-      <c r="D23" s="31" t="s">
-        <v>1096</v>
-      </c>
-      <c r="E23" s="31" t="s">
-        <v>1097</v>
-      </c>
-      <c r="F23" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="G23" s="12"/>
+    <row r="23" spans="1:13">
+      <c r="A23" s="12" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>1073</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>1074</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>964</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>1075</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>892</v>
+      </c>
       <c r="H23" s="12"/>
       <c r="I23" s="12"/>
       <c r="J23" s="12"/>
@@ -6749,31 +6783,27 @@
       <c r="L23" s="12"/>
       <c r="M23" s="12"/>
     </row>
-    <row r="24" spans="1:13">
-      <c r="A24" s="31" t="s">
-        <v>1098</v>
+    <row r="24" spans="1:13" ht="17">
+      <c r="A24" s="46" t="s">
+        <v>1093</v>
       </c>
       <c r="B24" s="31" t="s">
-        <v>1099</v>
+        <v>1094</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>26</v>
+        <v>1095</v>
       </c>
       <c r="D24" s="31" t="s">
-        <v>86</v>
+        <v>1096</v>
       </c>
       <c r="E24" s="31" t="s">
-        <v>1100</v>
+        <v>1097</v>
       </c>
       <c r="F24" s="31" t="s">
-        <v>1101</v>
-      </c>
-      <c r="G24" s="31" t="s">
-        <v>1102</v>
-      </c>
-      <c r="H24" s="31" t="s">
-        <v>1103</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
       <c r="I24" s="12"/>
       <c r="J24" s="12"/>
       <c r="K24" s="12"/>
@@ -6782,58 +6812,90 @@
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="31" t="s">
+        <v>1098</v>
+      </c>
+      <c r="B25" s="31" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C25" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="E25" s="31" t="s">
+        <v>1100</v>
+      </c>
+      <c r="F25" s="31" t="s">
+        <v>1101</v>
+      </c>
+      <c r="G25" s="31" t="s">
+        <v>1102</v>
+      </c>
+      <c r="H25" s="31" t="s">
+        <v>1103</v>
+      </c>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" s="31" t="s">
         <v>1104</v>
       </c>
-      <c r="B25" s="31" t="s">
+      <c r="B26" s="31" t="s">
         <v>1105</v>
       </c>
-      <c r="C25" s="31" t="s">
+      <c r="C26" s="31" t="s">
         <v>1106</v>
       </c>
-      <c r="D25" s="31" t="s">
+      <c r="D26" s="31" t="s">
         <v>1107</v>
       </c>
-      <c r="E25" s="31" t="s">
+      <c r="E26" s="31" t="s">
         <v>1108</v>
       </c>
-      <c r="F25" s="31" t="s">
+      <c r="F26" s="31" t="s">
         <v>1109</v>
       </c>
-      <c r="G25" s="31" t="s">
+      <c r="G26" s="31" t="s">
         <v>1110</v>
       </c>
-      <c r="H25" s="31" t="s">
+      <c r="H26" s="31" t="s">
         <v>1111</v>
       </c>
-      <c r="I25" s="31" t="s">
+      <c r="I26" s="31" t="s">
         <v>1112</v>
       </c>
-      <c r="J25" s="31" t="s">
+      <c r="J26" s="31" t="s">
         <v>1113</v>
       </c>
-      <c r="K25" s="31" t="s">
+      <c r="K26" s="31" t="s">
         <v>137</v>
       </c>
-      <c r="L25" s="31" t="s">
+      <c r="L26" s="31" t="s">
         <v>1114</v>
       </c>
-      <c r="M25" s="12"/>
+      <c r="M26" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:BC2"/>
   <sheetViews>
     <sheetView topLeftCell="AO1" workbookViewId="0">
       <selection activeCell="BC3" sqref="BC3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:55" s="20" customFormat="1" ht="34.5" customHeight="1">
       <c r="A1" s="40" t="s">
@@ -7062,20 +7124,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H111"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="3" width="9.140625" style="1" collapsed="1"/>
-    <col min="4" max="4" width="21.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="3" width="9.1640625" style="1" collapsed="1"/>
+    <col min="4" max="4" width="21.83203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.83203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.5" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="9.1640625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -9407,27 +9469,27 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:R111"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="I111" sqref="I2:I111"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-    <col min="2" max="2" width="18.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="19.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="9.1640625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="18.6640625" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.6640625" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19.33203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.83203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.33203125" style="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="13" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="27.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="17" width="9.140625" style="1" collapsed="1"/>
-    <col min="18" max="18" width="11.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="8" max="8" width="14.33203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="27.33203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="17" width="9.1640625" style="1" collapsed="1"/>
+    <col min="18" max="18" width="11.5" style="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="16384" width="9.1640625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -11355,7 +11417,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:R85"/>
+  <autoFilter ref="A1:R85" xr:uid="{00000000-0009-0000-0000-000005000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -11363,22 +11425,22 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:BC111"/>
   <sheetViews>
     <sheetView topLeftCell="AQ1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="AV1" sqref="AV1:BC1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.85546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.42578125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="18.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="15.33203125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.5" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.83203125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.83203125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9.1640625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.5" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="18.5" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:55" s="20" customFormat="1">
@@ -16968,24 +17030,24 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:F126"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="5.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.83203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75">
+    <row r="1" spans="1:6" ht="16">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
@@ -19284,23 +19346,23 @@
       <c r="F126" s="22"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F126"/>
+  <autoFilter ref="A1:F126" xr:uid="{00000000-0009-0000-0000-000007000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75">
+    <row r="1" spans="1:6" ht="16">
       <c r="A1" s="14" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
CSPLATFORM-2161 test cases added
</commit_message>
<xml_diff>
--- a/resources/excels/CD.xlsx
+++ b/resources/excels/CD.xlsx
@@ -5,37 +5,38 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a13221514/IdeaProjects/cs-portal-automation_selenium/resources/excels/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a13400947/Projects/cs-portal-automation_selenium/resources/excels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBED29ED-35DA-4843-AC25-06765552C7E4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51F7C9A5-4052-4F4A-8423-1D9477E9B8DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20480" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
     <sheet name=" Priority" sheetId="2" r:id="rId2"/>
     <sheet name="Headers" sheetId="3" r:id="rId3"/>
-    <sheet name="NFTRTickets-San" sheetId="4" r:id="rId4"/>
-    <sheet name="Assignment Rule" sheetId="22" r:id="rId5"/>
-    <sheet name="SLA Configuration" sheetId="21" r:id="rId6"/>
-    <sheet name="NFTRTickets-Reg" sheetId="11" r:id="rId7"/>
-    <sheet name="FTRTickets-Reg" sheetId="5" r:id="rId8"/>
-    <sheet name="FTRTickets-San" sheetId="12" r:id="rId9"/>
-    <sheet name="UserManagement" sheetId="13" r:id="rId10"/>
-    <sheet name="PinnedTags" sheetId="8" r:id="rId11"/>
-    <sheet name="Ticket State" sheetId="10" r:id="rId12"/>
-    <sheet name="TemplateManagement" sheetId="14" r:id="rId13"/>
-    <sheet name="Ticket Transfer Rules" sheetId="15" r:id="rId14"/>
-    <sheet name="Authentication Policy" sheetId="16" r:id="rId15"/>
-    <sheet name="Action Tagging" sheetId="17" r:id="rId16"/>
-    <sheet name="Transfer To Queue" sheetId="19" r:id="rId17"/>
-    <sheet name="QuestionAnswerKey" sheetId="20" r:id="rId18"/>
-    <sheet name="State Queue Mapping" sheetId="18" r:id="rId19"/>
+    <sheet name="OpenAPILoginSheet" sheetId="23" r:id="rId4"/>
+    <sheet name="NFTRTickets-San" sheetId="4" r:id="rId5"/>
+    <sheet name="Assignment Rule" sheetId="22" r:id="rId6"/>
+    <sheet name="SLA Configuration" sheetId="21" r:id="rId7"/>
+    <sheet name="NFTRTickets-Reg" sheetId="11" r:id="rId8"/>
+    <sheet name="FTRTickets-Reg" sheetId="5" r:id="rId9"/>
+    <sheet name="FTRTickets-San" sheetId="12" r:id="rId10"/>
+    <sheet name="UserManagement" sheetId="13" r:id="rId11"/>
+    <sheet name="PinnedTags" sheetId="8" r:id="rId12"/>
+    <sheet name="Ticket State" sheetId="10" r:id="rId13"/>
+    <sheet name="TemplateManagement" sheetId="14" r:id="rId14"/>
+    <sheet name="Ticket Transfer Rules" sheetId="15" r:id="rId15"/>
+    <sheet name="Authentication Policy" sheetId="16" r:id="rId16"/>
+    <sheet name="Action Tagging" sheetId="17" r:id="rId17"/>
+    <sheet name="Transfer To Queue" sheetId="19" r:id="rId18"/>
+    <sheet name="QuestionAnswerKey" sheetId="20" r:id="rId19"/>
+    <sheet name="State Queue Mapping" sheetId="18" r:id="rId20"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'FTRTickets-Reg'!$A$1:$F$126</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'SLA Configuration'!$A$1:$R$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'FTRTickets-Reg'!$A$1:$F$126</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'SLA Configuration'!$A$1:$R$1</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -498,7 +499,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3383" uniqueCount="1120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3390" uniqueCount="1127">
   <si>
     <t>loginAuuid</t>
   </si>
@@ -3866,13 +3867,34 @@
   <si>
     <t>Post balance
 (USD)</t>
+  </si>
+  <si>
+    <t>Token</t>
+  </si>
+  <si>
+    <t>API Type</t>
+  </si>
+  <si>
+    <t>Rest API</t>
+  </si>
+  <si>
+    <t>WKMh2WXamTTQtIrnkrC5/l9fCYOHhSa1hOgpKvmn5xZhNHkdTo8g7gpsGKiMXb/w3AjioDsIHk34HzJaReuqYUcHmN0KtpzrDoIHQ0cD0obcoZSykDm5lk55QPMbd20Vn3ZBFMDN4F9BYfxy98fwZXs+aUvM7wF6m2qunUhETMXh6NdTHBuJKtUMH7IE46UYg9h8k7UmWW8KkVjoyNuMii7OQUy6vMr+Y8CA4XGdqvFJ7ro9d9G87RjRl2YU0JG45DWmhKrb+fz7znkk7Q3o5ON5BZMEp+CXZ3cj8FJB4N6EO5ZAt4mEHUqrT/EbzZbjOVRnkrYtjRtudTn2/lJGxLSGoSUIVwxVkOCeJIHQusqWsb5R+Jf85rTmsKp+F//RZ8VzDxhL318YW4mF+fJGFeH29eGKFcqbwSBeAjizIpjxK3O1qcayBK+W7aVcsVU/UAFui5pdaE5loXhJ3rtuPQ==</t>
+  </si>
+  <si>
+    <t>OpenAPIValidToken</t>
+  </si>
+  <si>
+    <t>WKMh2WXamTTQtIrnkrC5/l9fCYOHhSa1hOgpKvmn5xZhNHkdTo8g7gpsGKiMXb/w3AjioDsIHk34HzJaReuqYUcHmN0KtpzrDoIHQ0cD0obcoZSykDm5lk55QPMbd20Vn3ZBFMDN4F9BYfxy98fwZXs+aUvM7wF6m2qunUhETMXh6NdTHBuJKtUMH7IE46UYg9h8k7UmWW8KkVjoyNuMii7OQUy6vMr+Y8CA4XGdqvFJ7ro9d9G87RjRl2YU0JG45DWmhKrb+fz7znkk7Q3o5ON5BZMEp+CXZ3cj8FJB4N6EO5ZAt4mEHUqrT/EbzZbjOVRnkrYtjRtudTn2/lJGxLSGoSUIVwxVkOCeJIHQusqWsb5R+Jf85rTmsKp+F//RZ8VzDxhL318YW4mF+fJGFeH29eGKFcqbwSBeAjizIpjxK3O1qcayBK+W7aVcsVU/UAFui5pdaE5loXhJ3rtu</t>
+  </si>
+  <si>
+    <t>OpenApiInvalidToken</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3967,6 +3989,13 @@
       <sz val="13"/>
       <color rgb="FF1C293B"/>
       <name val="Tondo-regular"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="9">
@@ -4124,7 +4153,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFill="1"/>
@@ -4192,6 +4221,9 @@
     <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4908,6 +4940,61 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16">
+      <c r="A1" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>491</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>492</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
@@ -5015,7 +5102,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -5122,7 +5209,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -5200,7 +5287,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -5266,7 +5353,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:E1"/>
   <sheetViews>
@@ -5306,7 +5393,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:M2"/>
   <sheetViews>
@@ -5406,7 +5493,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:J13"/>
   <sheetViews>
@@ -5658,7 +5745,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -5717,7 +5804,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:C15"/>
   <sheetViews>
@@ -5897,7 +5984,60 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="16">
+      <c r="A1" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
@@ -6018,64 +6158,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="16">
-      <c r="A1" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="11" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" s="11" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" s="11" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
@@ -6888,6 +6975,55 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5019A07-3447-304A-8B5F-11BFD86B8412}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="64" customWidth="1"/>
+    <col min="2" max="2" width="25.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17">
+      <c r="A1" s="47" t="s">
+        <v>1120</v>
+      </c>
+      <c r="B1" s="47" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17">
+      <c r="A2" s="47"/>
+      <c r="B2" s="47" t="s">
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="409.6">
+      <c r="A3" s="47" t="s">
+        <v>1123</v>
+      </c>
+      <c r="B3" s="47" t="s">
+        <v>1124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="409.6">
+      <c r="A4" s="47" t="s">
+        <v>1125</v>
+      </c>
+      <c r="B4" s="47" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:BC2"/>
   <sheetViews>
@@ -7123,7 +7259,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H111"/>
   <sheetViews>
@@ -9468,7 +9604,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:R111"/>
   <sheetViews>
@@ -11424,7 +11560,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:BC111"/>
   <sheetViews>
@@ -17029,7 +17165,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:F126"/>
   <sheetViews>
@@ -19350,59 +19486,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:6" ht="16">
-      <c r="A1" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>491</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>492</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="F2" s="22" t="s">
-        <v>68</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>